<commit_message>
Added latching circuit and fixed misc review catches
</commit_message>
<xml_diff>
--- a/Design_Calculations.xlsx
+++ b/Design_Calculations.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeth\Github\air-hockey-main-pcb-v1.x\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDEEB0AB-70D5-429D-8165-8089EF870DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AABCE2E-BC2A-4344-93B6-D0092AAA126E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-285" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E1062475-6C4E-4B1F-81DA-4BF6E08AD478}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{E1062475-6C4E-4B1F-81DA-4BF6E08AD478}"/>
   </bookViews>
   <sheets>
     <sheet name="INA225" sheetId="1" r:id="rId1"/>
-    <sheet name="Discharge" sheetId="2" r:id="rId2"/>
-    <sheet name="Current Budgeting" sheetId="3" r:id="rId3"/>
+    <sheet name="Shutdown Latch" sheetId="4" r:id="rId2"/>
+    <sheet name="Discharge" sheetId="2" r:id="rId3"/>
+    <sheet name="Current Budgeting" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
   <si>
     <t>V_supply</t>
   </si>
@@ -141,6 +141,33 @@
   </si>
   <si>
     <t>Total Net Current</t>
+  </si>
+  <si>
+    <t>Ra</t>
+  </si>
+  <si>
+    <t>Rb</t>
+  </si>
+  <si>
+    <t>Rc</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>Vo1</t>
+  </si>
+  <si>
+    <t>Vo2</t>
+  </si>
+  <si>
+    <t>ohms</t>
+  </si>
+  <si>
+    <t>volts</t>
+  </si>
+  <si>
+    <t>Rp</t>
   </si>
 </sst>
 </file>
@@ -156,12 +183,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -176,9 +209,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,13 +533,13 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -516,7 +550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -527,7 +561,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -538,7 +572,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -550,7 +584,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -562,7 +596,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -573,7 +607,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -585,7 +619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -596,7 +630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -611,7 +645,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -632,6 +666,198 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952D0EC4-E306-4640-ADE8-7AE534BFE6CA}">
+  <dimension ref="A1:J30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1">
+        <v>100000</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1">
+        <v>56000</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2">
+        <v>15000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2">
+        <v>10000</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3">
+        <v>3000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3">
+        <v>1000</v>
+      </c>
+      <c r="G3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6">
+        <f>1/((1/B2)+(1/B3))</f>
+        <v>2500</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6">
+        <f>1/((1/F2)+(1/F3))</f>
+        <v>909.09090909090901</v>
+      </c>
+      <c r="G6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7">
+        <f>B4*(B2/(B1+B2))</f>
+        <v>3.1304347826086953</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7">
+        <f>F4*(F2/(F1+F2))</f>
+        <v>3.6363636363636367</v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8">
+        <f>B4*(B6/(B6+B1))</f>
+        <v>0.58536585365853666</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8">
+        <f>F4*(F6/(F6+F1))</f>
+        <v>0.38338658146964855</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <f>5-1.9</f>
+        <v>3.1</v>
+      </c>
+      <c r="J29">
+        <f>5-3</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <f>I29/0.008</f>
+        <v>387.5</v>
+      </c>
+      <c r="J30">
+        <f>J29/0.008</f>
+        <v>250</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03A84CA0-770A-495D-B5C9-2F4450A807BE}">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -639,13 +865,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -656,7 +882,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -667,7 +893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -683,7 +909,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -694,7 +920,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -706,7 +932,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -717,7 +943,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -729,7 +955,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -746,23 +972,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D5E43B-C5E0-4F8F-99AA-47F1199742D4}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>

</xml_diff>